<commit_message>
Run with USDM package v0.61.0 (USDM v3.13.0)
</commit_message>
<xml_diff>
--- a/source_data/protocols/Alexion_NCT04573309_Wilsons/Alexion_NCT04573309_Wilsons.xlsx
+++ b/source_data/protocols/Alexion_NCT04573309_Wilsons/Alexion_NCT04573309_Wilsons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/Alexion_NCT04573309_Wilsons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45903C7-2D4B-994B-B587-4B745E0FFF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CE072F-88AD-4842-8BF3-F2DF7F8A35D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="49200" windowHeight="25420" firstSheet="18" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="49200" windowHeight="25420" firstSheet="19" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -7762,11 +7762,11 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -18332,7 +18332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF7CA68-BC48-5141-BEA0-B0ABEF929D94}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -18777,7 +18777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -19255,7 +19255,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="224" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="208" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>1149</v>
       </c>
@@ -19415,7 +19415,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="9" t="s">
         <v>1187</v>
       </c>
@@ -19450,7 +19450,7 @@
       </c>
       <c r="B84" s="40"/>
     </row>
-    <row r="85" spans="1:2" ht="288" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" ht="272" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
         <v>1195</v>
       </c>
@@ -22516,7 +22516,7 @@
       <c r="A1" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="54" t="s">
         <v>95</v>
       </c>
       <c r="C1" s="55"/>
@@ -22528,7 +22528,7 @@
       <c r="A2" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="54" t="s">
         <v>97</v>
       </c>
       <c r="C2" s="55"/>
@@ -22540,7 +22540,7 @@
       <c r="A3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="56" t="s">
         <v>99</v>
       </c>
       <c r="C3" s="55"/>
@@ -22552,7 +22552,7 @@
       <c r="A4" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="56" t="s">
         <v>101</v>
       </c>
       <c r="C4" s="55"/>
@@ -22564,7 +22564,7 @@
       <c r="A5" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="56" t="s">
         <v>103</v>
       </c>
       <c r="C5" s="55"/>
@@ -22576,7 +22576,7 @@
       <c r="A6" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="56" t="s">
         <v>105</v>
       </c>
       <c r="C6" s="55"/>
@@ -22588,7 +22588,7 @@
       <c r="A7" s="12" t="s">
         <v>1736</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="56" t="s">
         <v>106</v>
       </c>
       <c r="C7" s="55"/>
@@ -22600,7 +22600,7 @@
       <c r="A8" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="56" t="s">
         <v>108</v>
       </c>
       <c r="C8" s="55"/>
@@ -22612,7 +22612,7 @@
       <c r="A9" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="56" t="s">
         <v>110</v>
       </c>
       <c r="C9" s="55"/>
@@ -22624,7 +22624,7 @@
       <c r="A10" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="56" t="s">
         <v>112</v>
       </c>
       <c r="C10" s="55"/>
@@ -22636,7 +22636,7 @@
       <c r="A11" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="56" t="s">
         <v>113</v>
       </c>
       <c r="C11" s="55"/>
@@ -22648,7 +22648,7 @@
       <c r="A12" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="56" t="s">
         <v>115</v>
       </c>
       <c r="C12" s="55"/>
@@ -22660,7 +22660,7 @@
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="56" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="55"/>
@@ -22672,7 +22672,7 @@
       <c r="A14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="56" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="55"/>
@@ -22725,11 +22725,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B13:F13"/>
@@ -22739,6 +22734,11 @@
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>